<commit_message>
Fixed Von_ Bug in Verbindung CSV
</commit_message>
<xml_diff>
--- a/Excel and CSV Datenbank/Verbindung.xlsx
+++ b/Excel and CSV Datenbank/Verbindung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kien\Desktop\Seminar\Datenbank\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kien\Desktop\Seminar\Excel and CSV Datenbank\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,9 +32,6 @@
     <t>Dauer</t>
   </si>
   <si>
-    <t xml:space="preserve">Von </t>
-  </si>
-  <si>
     <t>Zu</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>V21</t>
+  </si>
+  <si>
+    <t>Von</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
   <tableColumns count="5">
     <tableColumn id="1" name="VNr"/>
     <tableColumn id="2" name="Dauer"/>
-    <tableColumn id="3" name="Von "/>
+    <tableColumn id="3" name="Von"/>
     <tableColumn id="4" name="Zu"/>
     <tableColumn id="5" name="Verkehrsart"/>
   </tableColumns>
@@ -499,7 +499,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -515,370 +515,370 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>38</v>
-      </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>